<commit_message>
Criação dos Graficos do powerBI
</commit_message>
<xml_diff>
--- a/PowerBI/kpis_mineracao.xlsx
+++ b/PowerBI/kpis_mineracao.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>id_maquina</t>
   </si>
@@ -65,33 +65,30 @@
     <t>Ana Souza</t>
   </si>
   <si>
+    <t>Sem ocorrencias</t>
+  </si>
+  <si>
+    <t>Caminhão Fora de Estrada</t>
+  </si>
+  <si>
+    <t>Em manutenção</t>
+  </si>
+  <si>
+    <t>Corretiva</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>7800.0</t>
+  </si>
+  <si>
+    <t>Britador Primário</t>
+  </si>
+  <si>
     <t>Preventiva</t>
   </si>
   <si>
-    <t>Sem ocorrências</t>
-  </si>
-  <si>
-    <t>3500.0</t>
-  </si>
-  <si>
-    <t>Caminhão Fora de Estrada</t>
-  </si>
-  <si>
-    <t>Em manutenção</t>
-  </si>
-  <si>
-    <t>Corretiva</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>7800.0</t>
-  </si>
-  <si>
-    <t>Britador Primário</t>
-  </si>
-  <si>
     <t>Média</t>
   </si>
   <si>
@@ -105,6 +102,24 @@
   </si>
   <si>
     <t>5600.0</t>
+  </si>
+  <si>
+    <t>caminhões de mineração</t>
+  </si>
+  <si>
+    <t>Inativa</t>
+  </si>
+  <si>
+    <t>Muito Alta</t>
+  </si>
+  <si>
+    <t>7000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perfuratrizes </t>
+  </si>
+  <si>
+    <t>6000.0</t>
   </si>
 </sst>
 </file>
@@ -117,13 +132,24 @@
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -590,141 +616,147 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1260,18 +1292,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="12.75" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="12.75" outlineLevelRow="7"/>
   <cols>
-    <col min="2" max="2" width="25.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="25.1428571428571" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="16.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="22.8571428571429" customWidth="1"/>
     <col min="8" max="8" width="20.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="19.1428571428571" customWidth="1"/>
   </cols>
@@ -1280,7 +1313,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1309,7 +1342,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -1322,53 +1355,53 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>43597</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>44046</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -1377,27 +1410,27 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>43148</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1406,19 +1439,106 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>44522</v>
       </c>
       <c r="I5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>45589</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>45658</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>45940</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>